<commit_message>
chaining of methods, pages, assertion
</commit_message>
<xml_diff>
--- a/AutomationProject/src/test/resources/TestData.xlsx
+++ b/AutomationProject/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mintu\git\NewRepo\AutomationProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EE059B-40D9-468A-9FBF-192C47C2159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEF984C-999B-4EC3-9598-E0C49E5B361C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>tiger</t>
-  </si>
-  <si>
     <t>duck</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>tom</t>
+  </si>
+  <si>
+    <t>ansul</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,7 +382,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -393,15 +393,15 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>